<commit_message>
Finish all use case except for admin use case
</commit_message>
<xml_diff>
--- a/NOVEMBER-2020.xlsx
+++ b/NOVEMBER-2020.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="54">
   <si>
     <t>TEAM</t>
   </si>
@@ -38,16 +38,37 @@
     <t>SUN 01/11</t>
   </si>
   <si>
+    <t>Long</t>
+  </si>
+  <si>
+    <t>08:00 - 16:00</t>
+  </si>
+  <si>
+    <t>08:00 - 17:00</t>
+  </si>
+  <si>
     <t>Hiếu</t>
   </si>
   <si>
-    <t>08:00 - 16:00</t>
-  </si>
-  <si>
-    <t>Long</t>
-  </si>
-  <si>
-    <t>08:00 - 17:00</t>
+    <t>13:00 - 19:00</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
   </si>
   <si>
     <t>MON 02/11</t>
@@ -1730,34 +1751,18 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="16" t="s">
-        <v>9</v>
-      </c>
+      <c r="A2" s="9"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="16"/>
     </row>
     <row r="3">
       <c r="A3" s="17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B3" s="18" t="s">
         <v>9</v>
@@ -1769,83 +1774,83 @@
         <v>9</v>
       </c>
       <c r="E3" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="24" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="25"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="32"/>
+      <c r="B4" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="32" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="33" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C7" s="35" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D7" s="36" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E7" s="37" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="F7" s="38" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="G7" s="39" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="H7" s="40" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="43" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="44" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="45" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="46" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" s="47" t="s">
-        <v>9</v>
-      </c>
-      <c r="H8" s="48" t="s">
-        <v>9</v>
-      </c>
+      <c r="A8" s="41"/>
+      <c r="B8" s="42"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="48"/>
     </row>
     <row r="9">
       <c r="A9" s="49" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B9" s="50" t="s">
         <v>9</v>
@@ -1857,83 +1862,83 @@
         <v>9</v>
       </c>
       <c r="E9" s="53" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="54" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="55" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="56" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="54" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="55" t="s">
-        <v>11</v>
-      </c>
-      <c r="H9" s="56" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="57"/>
-      <c r="B10" s="58"/>
-      <c r="C10" s="59"/>
-      <c r="D10" s="60"/>
-      <c r="E10" s="61"/>
-      <c r="F10" s="62"/>
-      <c r="G10" s="63"/>
-      <c r="H10" s="64"/>
+      <c r="B10" s="58" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="59" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="60" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="61" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="62" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="63" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="64" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="65" t="s">
         <v>0</v>
       </c>
       <c r="B13" s="66" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C13" s="67" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D13" s="68" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="E13" s="69" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="F13" s="70" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="G13" s="71" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="H13" s="72" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="73" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="74" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="75" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="76" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="77" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="78" t="s">
-        <v>9</v>
-      </c>
-      <c r="G14" s="79" t="s">
-        <v>9</v>
-      </c>
-      <c r="H14" s="80" t="s">
-        <v>9</v>
-      </c>
+      <c r="A14" s="73"/>
+      <c r="B14" s="74"/>
+      <c r="C14" s="75"/>
+      <c r="D14" s="76"/>
+      <c r="E14" s="77"/>
+      <c r="F14" s="78"/>
+      <c r="G14" s="79"/>
+      <c r="H14" s="80"/>
     </row>
     <row r="15">
       <c r="A15" s="81" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B15" s="82" t="s">
         <v>9</v>
@@ -1945,83 +1950,83 @@
         <v>9</v>
       </c>
       <c r="E15" s="85" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="86" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="87" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" s="88" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="89" t="s">
         <v>11</v>
       </c>
-      <c r="F15" s="86" t="s">
-        <v>11</v>
-      </c>
-      <c r="G15" s="87" t="s">
-        <v>11</v>
-      </c>
-      <c r="H15" s="88" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="89"/>
-      <c r="B16" s="90"/>
-      <c r="C16" s="91"/>
-      <c r="D16" s="92"/>
-      <c r="E16" s="93"/>
-      <c r="F16" s="94"/>
-      <c r="G16" s="95"/>
-      <c r="H16" s="96"/>
+      <c r="B16" s="90" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="91" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="92" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="93" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="94" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" s="95" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" s="96" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="97" t="s">
         <v>0</v>
       </c>
       <c r="B19" s="98" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C19" s="99" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="D19" s="100" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="E19" s="101" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="F19" s="102" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="G19" s="103" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="H19" s="104" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="105" t="s">
-        <v>8</v>
-      </c>
-      <c r="B20" s="106" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" s="107" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" s="108" t="s">
-        <v>9</v>
-      </c>
-      <c r="E20" s="109" t="s">
-        <v>9</v>
-      </c>
-      <c r="F20" s="110" t="s">
-        <v>9</v>
-      </c>
-      <c r="G20" s="111" t="s">
-        <v>9</v>
-      </c>
-      <c r="H20" s="112" t="s">
-        <v>9</v>
-      </c>
+      <c r="A20" s="105"/>
+      <c r="B20" s="106"/>
+      <c r="C20" s="107"/>
+      <c r="D20" s="108"/>
+      <c r="E20" s="109"/>
+      <c r="F20" s="110"/>
+      <c r="G20" s="111"/>
+      <c r="H20" s="112"/>
     </row>
     <row r="21">
       <c r="A21" s="113" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B21" s="114" t="s">
         <v>9</v>
@@ -2033,83 +2038,83 @@
         <v>9</v>
       </c>
       <c r="E21" s="117" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" s="118" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" s="119" t="s">
+        <v>10</v>
+      </c>
+      <c r="H21" s="120" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="121" t="s">
         <v>11</v>
       </c>
-      <c r="F21" s="118" t="s">
-        <v>11</v>
-      </c>
-      <c r="G21" s="119" t="s">
-        <v>11</v>
-      </c>
-      <c r="H21" s="120" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="121"/>
-      <c r="B22" s="122"/>
-      <c r="C22" s="123"/>
-      <c r="D22" s="124"/>
-      <c r="E22" s="125"/>
-      <c r="F22" s="126"/>
-      <c r="G22" s="127"/>
-      <c r="H22" s="128"/>
+      <c r="B22" s="122" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="123" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="124" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="125" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" s="126" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" s="127" t="s">
+        <v>17</v>
+      </c>
+      <c r="H22" s="128" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="129" t="s">
         <v>0</v>
       </c>
       <c r="B25" s="130" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C25" s="131" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="D25" s="132" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="E25" s="133" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="F25" s="134" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="G25" s="135" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="H25" s="136" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="137" t="s">
-        <v>8</v>
-      </c>
-      <c r="B26" s="138" t="s">
-        <v>9</v>
-      </c>
-      <c r="C26" s="139" t="s">
-        <v>9</v>
-      </c>
-      <c r="D26" s="140" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" s="141" t="s">
-        <v>9</v>
-      </c>
-      <c r="F26" s="142" t="s">
-        <v>9</v>
-      </c>
-      <c r="G26" s="143" t="s">
-        <v>9</v>
-      </c>
-      <c r="H26" s="144" t="s">
-        <v>9</v>
-      </c>
+      <c r="A26" s="137"/>
+      <c r="B26" s="138"/>
+      <c r="C26" s="139"/>
+      <c r="D26" s="140"/>
+      <c r="E26" s="141"/>
+      <c r="F26" s="142"/>
+      <c r="G26" s="143"/>
+      <c r="H26" s="144"/>
     </row>
     <row r="27">
       <c r="A27" s="145" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B27" s="146" t="s">
         <v>9</v>
@@ -2121,83 +2126,83 @@
         <v>9</v>
       </c>
       <c r="E27" s="149" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" s="150" t="s">
+        <v>10</v>
+      </c>
+      <c r="G27" s="151" t="s">
+        <v>10</v>
+      </c>
+      <c r="H27" s="152" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="153" t="s">
         <v>11</v>
       </c>
-      <c r="F27" s="150" t="s">
-        <v>11</v>
-      </c>
-      <c r="G27" s="151" t="s">
-        <v>11</v>
-      </c>
-      <c r="H27" s="152" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="153"/>
-      <c r="B28" s="154"/>
-      <c r="C28" s="155"/>
-      <c r="D28" s="156"/>
-      <c r="E28" s="157"/>
-      <c r="F28" s="158"/>
-      <c r="G28" s="159"/>
-      <c r="H28" s="160"/>
+      <c r="B28" s="154" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" s="155" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" s="156" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28" s="157" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28" s="158" t="s">
+        <v>16</v>
+      </c>
+      <c r="G28" s="159" t="s">
+        <v>17</v>
+      </c>
+      <c r="H28" s="160" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="161" t="s">
         <v>0</v>
       </c>
       <c r="B31" s="162" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C31" s="163" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="D31" s="164" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="E31" s="165" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="F31" s="166" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="G31" s="167" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="H31" s="168" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="169" t="s">
-        <v>8</v>
-      </c>
-      <c r="B32" s="170" t="s">
-        <v>9</v>
-      </c>
-      <c r="C32" s="171" t="s">
-        <v>9</v>
-      </c>
-      <c r="D32" s="172" t="s">
-        <v>9</v>
-      </c>
-      <c r="E32" s="173" t="s">
-        <v>9</v>
-      </c>
-      <c r="F32" s="174" t="s">
-        <v>9</v>
-      </c>
-      <c r="G32" s="175" t="s">
-        <v>9</v>
-      </c>
-      <c r="H32" s="176" t="s">
-        <v>9</v>
-      </c>
+      <c r="A32" s="169"/>
+      <c r="B32" s="170"/>
+      <c r="C32" s="171"/>
+      <c r="D32" s="172"/>
+      <c r="E32" s="173"/>
+      <c r="F32" s="174"/>
+      <c r="G32" s="175"/>
+      <c r="H32" s="176"/>
     </row>
     <row r="33">
       <c r="A33" s="177" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B33" s="178" t="s">
         <v>9</v>
@@ -2209,27 +2214,43 @@
         <v>9</v>
       </c>
       <c r="E33" s="181" t="s">
+        <v>10</v>
+      </c>
+      <c r="F33" s="182" t="s">
+        <v>10</v>
+      </c>
+      <c r="G33" s="183" t="s">
+        <v>10</v>
+      </c>
+      <c r="H33" s="184" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="185" t="s">
         <v>11</v>
       </c>
-      <c r="F33" s="182" t="s">
-        <v>11</v>
-      </c>
-      <c r="G33" s="183" t="s">
-        <v>11</v>
-      </c>
-      <c r="H33" s="184" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="185"/>
-      <c r="B34" s="186"/>
-      <c r="C34" s="187"/>
-      <c r="D34" s="188"/>
-      <c r="E34" s="189"/>
-      <c r="F34" s="190"/>
-      <c r="G34" s="191"/>
-      <c r="H34" s="192"/>
+      <c r="B34" s="186" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34" s="187" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34" s="188" t="s">
+        <v>14</v>
+      </c>
+      <c r="E34" s="189" t="s">
+        <v>15</v>
+      </c>
+      <c r="F34" s="190" t="s">
+        <v>16</v>
+      </c>
+      <c r="G34" s="191" t="s">
+        <v>17</v>
+      </c>
+      <c r="H34" s="192" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>